<commit_message>
Updated Smell Analysis Documentation
</commit_message>
<xml_diff>
--- a/Documentation/Group_16_Smells_Analysis.xlsx
+++ b/Documentation/Group_16_Smells_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\welcome\Desktop\Dal Coursework\Winter_2022\CSCI 5308\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{543E78AF-0F19-496C-9B93-3E64B5D80166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87081914-B5CC-4613-A64D-3D49B4633AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D627CF3C-7D3F-443A-A2B4-3623376BAF05}"/>
   </bookViews>
@@ -940,9 +940,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1012,95 +1009,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="26">
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="8"/>
-          <bgColor theme="8"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -1156,13 +1072,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1177,6 +1086,97 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="8"/>
+          <bgColor theme="8"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1257,30 +1257,30 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7DABE145-BB2A-4147-9A91-99AD482CB27E}" name="Table4" displayName="Table4" ref="A79:I136" totalsRowShown="0" headerRowDxfId="10" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7DABE145-BB2A-4147-9A91-99AD482CB27E}" name="Table4" displayName="Table4" ref="A79:I136" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A79:I136" xr:uid="{FA753889-D6C2-4B6E-B939-3B4CF45F50C5}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{EEC9EF43-1960-4FC8-8DF8-A2BF34648030}" name="Project Name" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{E3CAD0FD-0379-40EC-A5DE-D24359153BE0}" name="Package Name" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{3E518F39-6405-4C91-AC8E-EE83D30A58B4}" name="Type Name" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{8832A258-A6CC-4663-945E-49DC7221E9C6}" name="Method Name" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{0D5D2383-745E-410D-959C-3DF3415CAF72}" name="Smell Category" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{FCD38D56-DC6B-496B-87C4-0F73EC41C4C7}" name="Smell" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{099BB656-A7B8-4AD2-8B10-06B1560BE33B}" name="Cause of the Smell" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{F96A0E56-7CEF-4195-B8A0-C7C9913665DA}" name="Method start line no" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{912615F5-A0B3-4462-ACD4-152F19D85D11}" name="Rationale for Acceptance of Smell" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{EEC9EF43-1960-4FC8-8DF8-A2BF34648030}" name="Project Name" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{E3CAD0FD-0379-40EC-A5DE-D24359153BE0}" name="Package Name" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{3E518F39-6405-4C91-AC8E-EE83D30A58B4}" name="Type Name" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{8832A258-A6CC-4663-945E-49DC7221E9C6}" name="Method Name" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{0D5D2383-745E-410D-959C-3DF3415CAF72}" name="Smell Category" dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{FCD38D56-DC6B-496B-87C4-0F73EC41C4C7}" name="Smell" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{099BB656-A7B8-4AD2-8B10-06B1560BE33B}" name="Cause of the Smell" dataDxfId="10"/>
+    <tableColumn id="8" xr3:uid="{F96A0E56-7CEF-4195-B8A0-C7C9913665DA}" name="Method start line no" dataDxfId="9"/>
+    <tableColumn id="9" xr3:uid="{912615F5-A0B3-4462-ACD4-152F19D85D11}" name="Rationale for Acceptance of Smell" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B629A12F-C0D4-43EF-A22C-B072EC2F8523}" name="Table7" displayName="Table7" ref="A67:C73" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="17" tableBorderDxfId="18" totalsRowBorderDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B629A12F-C0D4-43EF-A22C-B072EC2F8523}" name="Table7" displayName="Table7" ref="A67:C73" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A67:C73" xr:uid="{2F024144-6B6A-47BF-8430-58FF90DC055A}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{AC3BDCB6-2DFF-4C30-A232-E21084877D36}" name="Smell Category" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{4C2D4644-2F34-418B-8DD7-DE14E9CE2302}" name="Smell" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{030A6088-C8EF-4BB1-B42F-D8D98DCCE0B5}" name="Number of Instance" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{AC3BDCB6-2DFF-4C30-A232-E21084877D36}" name="Smell Category" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4C2D4644-2F34-418B-8DD7-DE14E9CE2302}" name="Smell" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{030A6088-C8EF-4BB1-B42F-D8D98DCCE0B5}" name="Number of Instance" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1586,7 +1586,7 @@
   <dimension ref="A2:V136"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:V2"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1598,59 +1598,59 @@
     <col min="5" max="5" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="135" style="3" customWidth="1"/>
-    <col min="8" max="8" width="52.85546875" style="19" customWidth="1"/>
+    <col min="8" max="8" width="52.85546875" style="18" customWidth="1"/>
     <col min="9" max="9" width="79" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:22" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-    </row>
-    <row r="3" spans="1:22" s="17" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="16"/>
-      <c r="U3" s="16"/>
-      <c r="V3" s="16"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="40"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+    </row>
+    <row r="3" spans="1:22" s="16" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
     </row>
     <row r="4" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
@@ -1671,7 +1671,7 @@
       <c r="G4" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="H4" s="22">
+      <c r="H4" s="21">
         <v>46</v>
       </c>
     </row>
@@ -1758,1341 +1758,1341 @@
     </row>
     <row r="13" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:22" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
+      <c r="A15" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="26" t="s">
+      <c r="D15" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="26" t="s">
+      <c r="H15" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="26" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="20" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="28" t="s">
+    <row r="16" spans="1:22" s="19" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="E16" s="28" t="s">
+      <c r="D16" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="E16" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="28" t="s">
+      <c r="F16" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="G16" s="28" t="s">
+      <c r="G16" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="H16" s="28" t="s">
-        <v>122</v>
-      </c>
-      <c r="I16" s="28" t="s">
+      <c r="H16" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="I16" s="27" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="39" t="s">
+      <c r="A17" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="39" t="s">
+      <c r="C17" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="39" t="s">
+      <c r="D17" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="E17" s="39" t="s">
+      <c r="E17" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="39" t="s">
+      <c r="F17" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="H17" s="39">
+      <c r="H17" s="38">
         <v>56</v>
       </c>
-      <c r="I17" s="39" t="s">
+      <c r="I17" s="38" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="39" t="s">
+      <c r="A18" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="38" t="s">
         <v>126</v>
       </c>
-      <c r="H18" s="39">
+      <c r="H18" s="38">
         <v>102</v>
       </c>
-      <c r="I18" s="39" t="s">
+      <c r="I18" s="38" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="39" t="s">
+      <c r="A19" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="39" t="s">
+      <c r="D19" s="38" t="s">
         <v>123</v>
       </c>
-      <c r="E19" s="39" t="s">
+      <c r="E19" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="F19" s="39" t="s">
+      <c r="F19" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G19" s="39" t="s">
+      <c r="G19" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="H19" s="39">
+      <c r="H19" s="38">
         <v>19</v>
       </c>
-      <c r="I19" s="39" t="s">
+      <c r="I19" s="38" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="39" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="39" t="s">
+      <c r="A20" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="39" t="s">
+      <c r="C20" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="39" t="s">
+      <c r="E20" s="38" t="s">
         <v>86</v>
       </c>
-      <c r="F20" s="39" t="s">
+      <c r="F20" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="G20" s="39" t="s">
+      <c r="G20" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="H20" s="39">
+      <c r="H20" s="38">
         <v>137</v>
       </c>
-      <c r="I20" s="39" t="s">
+      <c r="I20" s="38" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="40" t="s">
+      <c r="A21" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="40" t="s">
+      <c r="C21" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="E21" s="40" t="s">
+      <c r="E21" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="40" t="s">
+      <c r="F21" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G21" s="40" t="s">
+      <c r="G21" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="H21" s="40">
+      <c r="H21" s="39">
         <v>46</v>
       </c>
-      <c r="I21" s="40" t="s">
+      <c r="I21" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="40" t="s">
+      <c r="A22" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="40" t="s">
+      <c r="C22" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="40" t="s">
+      <c r="F22" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G22" s="40" t="s">
+      <c r="G22" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="H22" s="40">
+      <c r="H22" s="39">
         <v>46</v>
       </c>
-      <c r="I22" s="40" t="s">
+      <c r="I22" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="40" t="s">
+      <c r="A23" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="40" t="s">
+      <c r="C23" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="E23" s="40" t="s">
+      <c r="E23" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F23" s="40" t="s">
+      <c r="F23" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G23" s="40" t="s">
+      <c r="G23" s="39" t="s">
         <v>134</v>
       </c>
-      <c r="H23" s="40">
+      <c r="H23" s="39">
         <v>32</v>
       </c>
-      <c r="I23" s="40" t="s">
+      <c r="I23" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B24" s="40" t="s">
+      <c r="A24" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="40" t="s">
+      <c r="C24" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="E24" s="40" t="s">
+      <c r="E24" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="40" t="s">
+      <c r="F24" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G24" s="40" t="s">
+      <c r="G24" s="39" t="s">
         <v>131</v>
       </c>
-      <c r="H24" s="40">
+      <c r="H24" s="39">
         <v>32</v>
       </c>
-      <c r="I24" s="40" t="s">
+      <c r="I24" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B25" s="40" t="s">
+      <c r="A25" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="40" t="s">
+      <c r="C25" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="E25" s="40" t="s">
+      <c r="E25" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="40" t="s">
+      <c r="F25" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G25" s="40" t="s">
+      <c r="G25" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="H25" s="40">
+      <c r="H25" s="39">
         <v>32</v>
       </c>
-      <c r="I25" s="40" t="s">
+      <c r="I25" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="40" t="s">
+      <c r="A26" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="40" t="s">
+      <c r="C26" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="40" t="s">
+      <c r="F26" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G26" s="40" t="s">
+      <c r="G26" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="H26" s="40">
+      <c r="H26" s="39">
         <v>22</v>
       </c>
-      <c r="I26" s="40" t="s">
+      <c r="I26" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B27" s="40" t="s">
+      <c r="A27" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="40" t="s">
+      <c r="C27" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="E27" s="40" t="s">
+      <c r="E27" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="40" t="s">
+      <c r="F27" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G27" s="40" t="s">
+      <c r="G27" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="H27" s="40">
+      <c r="H27" s="39">
         <v>38</v>
       </c>
-      <c r="I27" s="40" t="s">
+      <c r="I27" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B28" s="40" t="s">
+      <c r="A28" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C28" s="40" t="s">
+      <c r="C28" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="E28" s="40" t="s">
+      <c r="E28" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="40" t="s">
+      <c r="F28" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G28" s="40" t="s">
+      <c r="G28" s="39" t="s">
         <v>140</v>
       </c>
-      <c r="H28" s="40">
+      <c r="H28" s="39">
         <v>24</v>
       </c>
-      <c r="I28" s="40" t="s">
+      <c r="I28" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="40" t="s">
+      <c r="A29" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="40" t="s">
+      <c r="C29" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="E29" s="40" t="s">
+      <c r="E29" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F29" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G29" s="40" t="s">
+      <c r="G29" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="H29" s="40">
+      <c r="H29" s="39">
         <v>38</v>
       </c>
-      <c r="I29" s="40" t="s">
+      <c r="I29" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="40" t="s">
+      <c r="A30" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="40" t="s">
+      <c r="C30" s="39" t="s">
         <v>52</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="39" t="s">
         <v>143</v>
       </c>
-      <c r="E30" s="40" t="s">
+      <c r="E30" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F30" s="40" t="s">
+      <c r="F30" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G30" s="40" t="s">
+      <c r="G30" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="H30" s="40">
+      <c r="H30" s="39">
         <v>68</v>
       </c>
-      <c r="I30" s="40" t="s">
+      <c r="I30" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B31" s="40" t="s">
+      <c r="A31" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="E31" s="40" t="s">
+      <c r="E31" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F31" s="40" t="s">
+      <c r="F31" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G31" s="40" t="s">
+      <c r="G31" s="39" t="s">
         <v>146</v>
       </c>
-      <c r="H31" s="40">
-        <v>20</v>
-      </c>
-      <c r="I31" s="40" t="s">
+      <c r="H31" s="39">
+        <v>20</v>
+      </c>
+      <c r="I31" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B32" s="40" t="s">
+      <c r="A32" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="40" t="s">
+      <c r="C32" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="E32" s="40" t="s">
+      <c r="E32" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F32" s="40" t="s">
+      <c r="F32" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G32" s="40" t="s">
+      <c r="G32" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="H32" s="40">
+      <c r="H32" s="39">
         <v>28</v>
       </c>
-      <c r="I32" s="40" t="s">
+      <c r="I32" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B33" s="40" t="s">
+      <c r="A33" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="40" t="s">
+      <c r="C33" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="40" t="s">
+      <c r="D33" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="E33" s="40" t="s">
+      <c r="E33" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F33" s="40" t="s">
+      <c r="F33" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G33" s="40" t="s">
+      <c r="G33" s="39" t="s">
         <v>149</v>
       </c>
-      <c r="H33" s="40">
+      <c r="H33" s="39">
         <v>102</v>
       </c>
-      <c r="I33" s="40" t="s">
+      <c r="I33" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B34" s="40" t="s">
+      <c r="A34" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="40" t="s">
+      <c r="C34" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="E34" s="40" t="s">
+      <c r="E34" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F34" s="40" t="s">
+      <c r="F34" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G34" s="40" t="s">
+      <c r="G34" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="H34" s="40">
+      <c r="H34" s="39">
         <v>102</v>
       </c>
-      <c r="I34" s="40" t="s">
+      <c r="I34" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35" s="40" t="s">
+      <c r="A35" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="40" t="s">
+      <c r="C35" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D35" s="40" t="s">
+      <c r="D35" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="E35" s="40" t="s">
+      <c r="E35" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F35" s="40" t="s">
+      <c r="F35" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G35" s="40" t="s">
+      <c r="G35" s="39" t="s">
         <v>152</v>
       </c>
-      <c r="H35" s="40">
+      <c r="H35" s="39">
         <v>22</v>
       </c>
-      <c r="I35" s="40" t="s">
+      <c r="I35" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B36" s="40" t="s">
+      <c r="A36" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="40" t="s">
+      <c r="C36" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="40" t="s">
+      <c r="D36" s="39" t="s">
         <v>153</v>
       </c>
-      <c r="E36" s="40" t="s">
+      <c r="E36" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F36" s="40" t="s">
+      <c r="F36" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G36" s="40" t="s">
+      <c r="G36" s="39" t="s">
         <v>154</v>
       </c>
-      <c r="H36" s="40">
+      <c r="H36" s="39">
         <v>40</v>
       </c>
-      <c r="I36" s="40" t="s">
+      <c r="I36" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B37" s="40" t="s">
+      <c r="A37" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="40" t="s">
+      <c r="C37" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D37" s="40" t="s">
+      <c r="D37" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F37" s="40" t="s">
+      <c r="F37" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G37" s="40" t="s">
+      <c r="G37" s="39" t="s">
         <v>156</v>
       </c>
-      <c r="H37" s="40">
+      <c r="H37" s="39">
         <v>65</v>
       </c>
-      <c r="I37" s="40" t="s">
+      <c r="I37" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B38" s="40" t="s">
+      <c r="A38" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="40" t="s">
+      <c r="D38" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F38" s="40" t="s">
+      <c r="F38" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G38" s="40" t="s">
+      <c r="G38" s="39" t="s">
         <v>158</v>
       </c>
-      <c r="H38" s="40">
+      <c r="H38" s="39">
         <v>81</v>
       </c>
-      <c r="I38" s="40" t="s">
+      <c r="I38" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B39" s="40" t="s">
+      <c r="A39" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="40" t="s">
+      <c r="C39" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="40" t="s">
+      <c r="D39" s="39" t="s">
         <v>159</v>
       </c>
-      <c r="E39" s="40" t="s">
+      <c r="E39" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F39" s="40" t="s">
+      <c r="F39" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G39" s="40" t="s">
+      <c r="G39" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="H39" s="40">
+      <c r="H39" s="39">
         <v>22</v>
       </c>
-      <c r="I39" s="40" t="s">
+      <c r="I39" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="40" t="s">
+      <c r="A40" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="40" t="s">
+      <c r="C40" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="D40" s="40" t="s">
+      <c r="D40" s="39" t="s">
         <v>161</v>
       </c>
-      <c r="E40" s="40" t="s">
+      <c r="E40" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F40" s="40" t="s">
+      <c r="F40" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G40" s="40" t="s">
+      <c r="G40" s="39" t="s">
         <v>162</v>
       </c>
-      <c r="H40" s="40">
+      <c r="H40" s="39">
         <v>36</v>
       </c>
-      <c r="I40" s="40" t="s">
+      <c r="I40" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="40" t="s">
+      <c r="A41" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="40" t="s">
+      <c r="C41" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="40" t="s">
+      <c r="D41" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="E41" s="40" t="s">
+      <c r="E41" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F41" s="40" t="s">
+      <c r="F41" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G41" s="40" t="s">
+      <c r="G41" s="39" t="s">
         <v>164</v>
       </c>
-      <c r="H41" s="40">
+      <c r="H41" s="39">
         <v>51</v>
       </c>
-      <c r="I41" s="40" t="s">
+      <c r="I41" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A42" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B42" s="40" t="s">
+      <c r="A42" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C42" s="40" t="s">
+      <c r="C42" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D42" s="39" t="s">
         <v>165</v>
       </c>
-      <c r="E42" s="40" t="s">
+      <c r="E42" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F42" s="40" t="s">
+      <c r="F42" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G42" s="40" t="s">
+      <c r="G42" s="39" t="s">
         <v>166</v>
       </c>
-      <c r="H42" s="40">
+      <c r="H42" s="39">
         <v>67</v>
       </c>
-      <c r="I42" s="40" t="s">
+      <c r="I42" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43" s="40" t="s">
+      <c r="A43" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="40" t="s">
+      <c r="C43" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D43" s="40" t="s">
+      <c r="D43" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="E43" s="40" t="s">
+      <c r="E43" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F43" s="40" t="s">
+      <c r="F43" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G43" s="40" t="s">
+      <c r="G43" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="H43" s="40">
+      <c r="H43" s="39">
         <v>26</v>
       </c>
-      <c r="I43" s="40" t="s">
+      <c r="I43" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B44" s="40" t="s">
+      <c r="A44" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="40" t="s">
+      <c r="C44" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D44" s="40" t="s">
+      <c r="D44" s="39" t="s">
         <v>169</v>
       </c>
-      <c r="E44" s="40" t="s">
+      <c r="E44" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F44" s="40" t="s">
+      <c r="F44" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G44" s="40" t="s">
+      <c r="G44" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="H44" s="40">
+      <c r="H44" s="39">
         <v>42</v>
       </c>
-      <c r="I44" s="40" t="s">
+      <c r="I44" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B45" s="40" t="s">
+      <c r="A45" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C45" s="40" t="s">
+      <c r="C45" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="D45" s="40" t="s">
+      <c r="D45" s="39" t="s">
         <v>171</v>
       </c>
-      <c r="E45" s="40" t="s">
+      <c r="E45" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F45" s="40" t="s">
+      <c r="F45" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G45" s="40" t="s">
+      <c r="G45" s="39" t="s">
         <v>172</v>
       </c>
-      <c r="H45" s="40">
+      <c r="H45" s="39">
         <v>73</v>
       </c>
-      <c r="I45" s="40" t="s">
+      <c r="I45" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B46" s="40" t="s">
+      <c r="A46" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B46" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="40" t="s">
+      <c r="C46" s="39" t="s">
         <v>84</v>
       </c>
-      <c r="D46" s="40" t="s">
+      <c r="D46" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="E46" s="40" t="s">
+      <c r="E46" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F46" s="40" t="s">
+      <c r="F46" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G46" s="40" t="s">
+      <c r="G46" s="39" t="s">
         <v>174</v>
       </c>
-      <c r="H46" s="40">
+      <c r="H46" s="39">
         <v>114</v>
       </c>
-      <c r="I46" s="40" t="s">
+      <c r="I46" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B47" s="40" t="s">
+      <c r="A47" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B47" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="40" t="s">
+      <c r="C47" s="39" t="s">
         <v>82</v>
       </c>
-      <c r="D47" s="40" t="s">
+      <c r="D47" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="E47" s="40" t="s">
+      <c r="E47" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F47" s="40" t="s">
+      <c r="F47" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G47" s="40" t="s">
+      <c r="G47" s="39" t="s">
         <v>175</v>
       </c>
-      <c r="H47" s="40">
+      <c r="H47" s="39">
         <v>105</v>
       </c>
-      <c r="I47" s="40" t="s">
+      <c r="I47" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" s="40" t="s">
+      <c r="A48" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="40" t="s">
+      <c r="C48" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="D48" s="40" t="s">
+      <c r="D48" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="E48" s="40" t="s">
+      <c r="E48" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F48" s="40" t="s">
+      <c r="F48" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G48" s="40" t="s">
+      <c r="G48" s="39" t="s">
         <v>176</v>
       </c>
-      <c r="H48" s="40">
+      <c r="H48" s="39">
         <v>108</v>
       </c>
-      <c r="I48" s="40" t="s">
+      <c r="I48" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B49" s="40" t="s">
+      <c r="A49" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B49" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C49" s="40" t="s">
+      <c r="C49" s="39" t="s">
         <v>177</v>
       </c>
-      <c r="D49" s="40" t="s">
+      <c r="D49" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="E49" s="40" t="s">
+      <c r="E49" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F49" s="40" t="s">
+      <c r="F49" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G49" s="40" t="s">
+      <c r="G49" s="39" t="s">
         <v>178</v>
       </c>
-      <c r="H49" s="40">
+      <c r="H49" s="39">
         <v>90</v>
       </c>
-      <c r="I49" s="40" t="s">
+      <c r="I49" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B50" s="40" t="s">
+      <c r="A50" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B50" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C50" s="40" t="s">
+      <c r="C50" s="39" t="s">
         <v>64</v>
       </c>
-      <c r="D50" s="40" t="s">
+      <c r="D50" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="E50" s="40" t="s">
+      <c r="E50" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F50" s="40" t="s">
+      <c r="F50" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G50" s="40" t="s">
+      <c r="G50" s="39" t="s">
         <v>179</v>
       </c>
-      <c r="H50" s="40">
+      <c r="H50" s="39">
         <v>163</v>
       </c>
-      <c r="I50" s="40" t="s">
+      <c r="I50" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B51" s="40" t="s">
+      <c r="A51" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B51" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="40" t="s">
+      <c r="C51" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="D51" s="40" t="s">
+      <c r="D51" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="E51" s="40" t="s">
+      <c r="E51" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F51" s="40" t="s">
+      <c r="F51" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G51" s="40" t="s">
+      <c r="G51" s="39" t="s">
         <v>180</v>
       </c>
-      <c r="H51" s="40">
+      <c r="H51" s="39">
         <v>174</v>
       </c>
-      <c r="I51" s="40" t="s">
+      <c r="I51" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B52" s="40" t="s">
+      <c r="A52" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B52" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="C52" s="40" t="s">
+      <c r="C52" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="D52" s="40" t="s">
+      <c r="D52" s="39" t="s">
         <v>173</v>
       </c>
-      <c r="E52" s="40" t="s">
+      <c r="E52" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F52" s="40" t="s">
+      <c r="F52" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G52" s="40" t="s">
+      <c r="G52" s="39" t="s">
         <v>181</v>
       </c>
-      <c r="H52" s="40">
+      <c r="H52" s="39">
         <v>102</v>
       </c>
-      <c r="I52" s="40" t="s">
+      <c r="I52" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B53" s="40" t="s">
+      <c r="A53" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B53" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C53" s="40" t="s">
+      <c r="C53" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D53" s="40" t="s">
+      <c r="D53" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="E53" s="40" t="s">
+      <c r="E53" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F53" s="40" t="s">
+      <c r="F53" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G53" s="40" t="s">
+      <c r="G53" s="39" t="s">
         <v>182</v>
       </c>
-      <c r="H53" s="40">
+      <c r="H53" s="39">
         <v>48</v>
       </c>
-      <c r="I53" s="40" t="s">
+      <c r="I53" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A54" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B54" s="40" t="s">
+      <c r="A54" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B54" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C54" s="40" t="s">
+      <c r="C54" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D54" s="40" t="s">
+      <c r="D54" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="E54" s="40" t="s">
+      <c r="E54" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F54" s="40" t="s">
+      <c r="F54" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G54" s="40" t="s">
+      <c r="G54" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="H54" s="40">
+      <c r="H54" s="39">
         <v>131</v>
       </c>
-      <c r="I54" s="40" t="s">
+      <c r="I54" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B55" s="40" t="s">
+      <c r="A55" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B55" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C55" s="40" t="s">
+      <c r="C55" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="D55" s="40" t="s">
+      <c r="D55" s="39" t="s">
         <v>183</v>
       </c>
-      <c r="E55" s="40" t="s">
+      <c r="E55" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F55" s="40" t="s">
+      <c r="F55" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G55" s="40" t="s">
+      <c r="G55" s="39" t="s">
         <v>185</v>
       </c>
-      <c r="H55" s="40">
+      <c r="H55" s="39">
         <v>131</v>
       </c>
-      <c r="I55" s="40" t="s">
+      <c r="I55" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B56" s="40" t="s">
+      <c r="A56" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C56" s="40" t="s">
+      <c r="C56" s="39" t="s">
         <v>33</v>
       </c>
-      <c r="D56" s="40" t="s">
+      <c r="D56" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="E56" s="40" t="s">
+      <c r="E56" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F56" s="40" t="s">
+      <c r="F56" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G56" s="40" t="s">
+      <c r="G56" s="39" t="s">
         <v>186</v>
       </c>
-      <c r="H56" s="40">
+      <c r="H56" s="39">
         <v>22</v>
       </c>
-      <c r="I56" s="40" t="s">
+      <c r="I56" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B57" s="40" t="s">
+      <c r="A57" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B57" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C57" s="40" t="s">
+      <c r="C57" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D57" s="40" t="s">
+      <c r="D57" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="E57" s="40" t="s">
+      <c r="E57" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F57" s="40" t="s">
+      <c r="F57" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G57" s="40" t="s">
+      <c r="G57" s="39" t="s">
         <v>187</v>
       </c>
-      <c r="H57" s="40">
+      <c r="H57" s="39">
         <v>39</v>
       </c>
-      <c r="I57" s="40" t="s">
+      <c r="I57" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B58" s="40" t="s">
+      <c r="A58" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B58" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C58" s="40" t="s">
+      <c r="C58" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D58" s="40" t="s">
+      <c r="D58" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="E58" s="40" t="s">
+      <c r="E58" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F58" s="40" t="s">
+      <c r="F58" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G58" s="40" t="s">
+      <c r="G58" s="39" t="s">
         <v>188</v>
       </c>
-      <c r="H58" s="40">
+      <c r="H58" s="39">
         <v>103</v>
       </c>
-      <c r="I58" s="40" t="s">
+      <c r="I58" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B59" s="40" t="s">
+      <c r="A59" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B59" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C59" s="40" t="s">
+      <c r="C59" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="D59" s="40" t="s">
+      <c r="D59" s="39" t="s">
         <v>155</v>
       </c>
-      <c r="E59" s="40" t="s">
+      <c r="E59" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F59" s="40" t="s">
+      <c r="F59" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G59" s="40" t="s">
+      <c r="G59" s="39" t="s">
         <v>189</v>
       </c>
-      <c r="H59" s="40">
+      <c r="H59" s="39">
         <v>103</v>
       </c>
-      <c r="I59" s="40" t="s">
+      <c r="I59" s="39" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="B60" s="40" t="s">
+      <c r="A60" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B60" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="C60" s="40" t="s">
+      <c r="C60" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="D60" s="40" t="s">
+      <c r="D60" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="E60" s="40" t="s">
+      <c r="E60" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="F60" s="40" t="s">
+      <c r="F60" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="G60" s="40" t="s">
+      <c r="G60" s="39" t="s">
         <v>190</v>
       </c>
-      <c r="H60" s="40">
-        <v>21</v>
-      </c>
-      <c r="I60" s="40" t="s">
+      <c r="H60" s="39">
+        <v>21</v>
+      </c>
+      <c r="I60" s="39" t="s">
         <v>191</v>
       </c>
     </row>
@@ -3102,114 +3102,114 @@
       </c>
     </row>
     <row r="67" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="29" t="s">
+      <c r="A67" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="B67" s="29" t="s">
         <v>98</v>
       </c>
-      <c r="C67" s="31" t="s">
+      <c r="C67" s="30" t="s">
         <v>101</v>
       </c>
       <c r="E67" s="6"/>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="32" t="s">
+      <c r="A68" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="B68" s="33" t="s">
+      <c r="B68" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="34">
+      <c r="C68" s="33">
         <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="32" t="s">
+      <c r="A69" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B69" s="33" t="s">
+      <c r="B69" s="32" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="34">
+      <c r="C69" s="33">
         <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="32" t="s">
+      <c r="A70" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B70" s="33" t="s">
+      <c r="B70" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C70" s="34">
+      <c r="C70" s="33">
         <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="32" t="s">
+      <c r="A71" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B71" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="C71" s="34">
+      <c r="B71" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" s="33">
         <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="32" t="s">
+      <c r="A72" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="B72" s="33" t="s">
+      <c r="B72" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C72" s="34">
+      <c r="C72" s="33">
         <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="35" t="s">
+      <c r="A73" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="B73" s="36" t="s">
+      <c r="B73" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="C73" s="37">
+      <c r="C73" s="36">
         <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A78" s="24" t="s">
+      <c r="A78" s="23" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A79" s="23" t="s">
+      <c r="A79" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B79" s="23" t="s">
+      <c r="B79" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C79" s="23" t="s">
+      <c r="C79" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D79" s="23" t="s">
+      <c r="D79" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="E79" s="23" t="s">
+      <c r="E79" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="F79" s="23" t="s">
+      <c r="F79" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="G79" s="23" t="s">
+      <c r="G79" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H79" s="23" t="s">
+      <c r="H79" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="I79" s="23" t="s">
+      <c r="I79" s="22" t="s">
         <v>97</v>
       </c>
     </row>
@@ -3235,7 +3235,7 @@
       <c r="G80" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="H80" s="38">
+      <c r="H80" s="37">
         <v>39</v>
       </c>
       <c r="I80" s="14" t="s">
@@ -3264,7 +3264,7 @@
       <c r="G81" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="H81" s="38">
+      <c r="H81" s="37">
         <v>37</v>
       </c>
       <c r="I81" s="14" t="s">
@@ -3293,7 +3293,7 @@
       <c r="G82" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="H82" s="38">
+      <c r="H82" s="37">
         <v>42</v>
       </c>
       <c r="I82" s="14" t="s">
@@ -3322,7 +3322,7 @@
       <c r="G83" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="H83" s="38">
+      <c r="H83" s="37">
         <v>14</v>
       </c>
       <c r="I83" s="14" t="s">
@@ -3351,7 +3351,7 @@
       <c r="G84" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="H84" s="38">
+      <c r="H84" s="37">
         <v>47</v>
       </c>
       <c r="I84" s="14" t="s">
@@ -3380,7 +3380,7 @@
       <c r="G85" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="H85" s="38">
+      <c r="H85" s="37">
         <v>55</v>
       </c>
       <c r="I85" s="14" t="s">
@@ -3409,7 +3409,7 @@
       <c r="G86" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="H86" s="38">
+      <c r="H86" s="37">
         <v>36</v>
       </c>
       <c r="I86" s="14" t="s">
@@ -3417,147 +3417,147 @@
       </c>
     </row>
     <row r="87" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B87" s="38" t="s">
+      <c r="A87" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B87" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C87" s="38" t="s">
+      <c r="C87" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="D87" s="38" t="s">
+      <c r="D87" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="E87" s="38" t="s">
+      <c r="E87" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F87" s="38" t="s">
+      <c r="F87" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G87" s="38" t="s">
+      <c r="G87" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="H87" s="38">
+      <c r="H87" s="37">
         <v>153</v>
       </c>
-      <c r="I87" s="38" t="s">
+      <c r="I87" s="37" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B88" s="38" t="s">
+      <c r="A88" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B88" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C88" s="38" t="s">
+      <c r="C88" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D88" s="38" t="s">
+      <c r="D88" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E88" s="38" t="s">
+      <c r="E88" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F88" s="38" t="s">
+      <c r="F88" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G88" s="38" t="s">
+      <c r="G88" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="H88" s="38">
+      <c r="H88" s="37">
         <v>107</v>
       </c>
-      <c r="I88" s="38" t="s">
+      <c r="I88" s="37" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B89" s="38" t="s">
+      <c r="A89" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C89" s="38" t="s">
+      <c r="C89" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D89" s="38" t="s">
+      <c r="D89" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="E89" s="38" t="s">
+      <c r="E89" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F89" s="38" t="s">
+      <c r="F89" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G89" s="38" t="s">
+      <c r="G89" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="H89" s="38">
+      <c r="H89" s="37">
         <v>107</v>
       </c>
-      <c r="I89" s="38" t="s">
+      <c r="I89" s="37" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A90" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B90" s="38" t="s">
+      <c r="A90" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B90" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C90" s="38" t="s">
+      <c r="C90" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D90" s="38" t="s">
+      <c r="D90" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E90" s="38" t="s">
+      <c r="E90" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F90" s="38" t="s">
+      <c r="F90" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G90" s="38" t="s">
+      <c r="G90" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="H90" s="38">
+      <c r="H90" s="37">
         <v>116</v>
       </c>
-      <c r="I90" s="38" t="s">
+      <c r="I90" s="37" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A91" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="B91" s="38" t="s">
+      <c r="A91" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B91" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C91" s="38" t="s">
+      <c r="C91" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="D91" s="38" t="s">
+      <c r="D91" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E91" s="38" t="s">
+      <c r="E91" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="F91" s="38" t="s">
+      <c r="F91" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="G91" s="38" t="s">
+      <c r="G91" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H91" s="38">
+      <c r="H91" s="37">
         <v>116</v>
       </c>
-      <c r="I91" s="38" t="s">
+      <c r="I91" s="37" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>